<commit_message>
Ashish's FTIR figures, meeting with Ashish, formatting Vmax data for Ashish
Ashish sent me FTIR figures. I also met with Ashish on Thursday May 15, 2024. Finally, I log10-transformed the Vmax data and then formatted it according to how he wants it.
</commit_message>
<xml_diff>
--- a/CAZyme metagenomic data/CAZyme TPM substrates brian.xlsx
+++ b/CAZyme metagenomic data/CAZyme TPM substrates brian.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s18am9/Library/Mobile Documents/com~apple~CloudDocs/Documents/UCI/DNA Work_Seasonal/Assembly work/CAZyme/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LMAOXD\Documents\UCI undergrad\Bio-ESS 199\Microbial-enzyme-activity-in-leaf-litter\CAZyme metagenomic data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F089493-01B3-4D47-9BD3-A853078EC139}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30C8E1CD-9B0D-4C2E-B04E-EFB68EFA3E5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37980" yWindow="-5060" windowWidth="37860" windowHeight="19380" xr2:uid="{87346394-57BB-9949-AE39-A726742C3854}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{87346394-57BB-9949-AE39-A726742C3854}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet4" sheetId="4" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet4!$C$1:$C$348</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet4!$A$1:$BO$348</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1976,12 +1976,15 @@
   <dimension ref="A1:BO348"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A350" sqref="A350:XFD350"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="124.3984375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2184,7 +2187,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="2" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2387,7 +2390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2590,7 +2593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2793,7 +2796,7 @@
         <v>415.660884006125</v>
       </c>
     </row>
-    <row r="5" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2996,7 +2999,7 @@
         <v>1344.56100940537</v>
       </c>
     </row>
-    <row r="6" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -3199,7 +3202,7 @@
         <v>3746.4131542946302</v>
       </c>
     </row>
-    <row r="7" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -3402,7 +3405,7 @@
         <v>6130.60676139923</v>
       </c>
     </row>
-    <row r="8" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -3605,7 +3608,7 @@
         <v>142.4643668718</v>
       </c>
     </row>
-    <row r="9" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -3808,7 +3811,7 @@
         <v>7684.7531171398996</v>
       </c>
     </row>
-    <row r="10" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -4011,7 +4014,7 @@
         <v>45.0739763904349</v>
       </c>
     </row>
-    <row r="11" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -4214,7 +4217,7 @@
         <v>111.530308215525</v>
       </c>
     </row>
-    <row r="12" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -4417,7 +4420,7 @@
         <v>3391.2296746084899</v>
       </c>
     </row>
-    <row r="13" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -4620,7 +4623,7 @@
         <v>273.34443991138698</v>
       </c>
     </row>
-    <row r="14" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -4823,7 +4826,7 @@
         <v>214.29998997145401</v>
       </c>
     </row>
-    <row r="15" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -5026,7 +5029,7 @@
         <v>171.22580625978699</v>
       </c>
     </row>
-    <row r="16" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -5229,7 +5232,7 @@
         <v>5758.5526831075604</v>
       </c>
     </row>
-    <row r="17" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -5432,7 +5435,7 @@
         <v>8533.08671494394</v>
       </c>
     </row>
-    <row r="18" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -5635,7 +5638,7 @@
         <v>307.61359382925701</v>
       </c>
     </row>
-    <row r="19" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -5838,7 +5841,7 @@
         <v>1478.4123525078501</v>
       </c>
     </row>
-    <row r="20" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -6041,7 +6044,7 @@
         <v>101.73323185311</v>
       </c>
     </row>
-    <row r="21" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -6244,7 +6247,7 @@
         <v>681.01606774337301</v>
       </c>
     </row>
-    <row r="22" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -6447,7 +6450,7 @@
         <v>2057.0862239755402</v>
       </c>
     </row>
-    <row r="23" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -6650,7 +6653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -6853,7 +6856,7 @@
         <v>57.394360004133603</v>
       </c>
     </row>
-    <row r="25" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -7056,7 +7059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -7259,7 +7262,7 @@
         <v>144.81134920984599</v>
       </c>
     </row>
-    <row r="27" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -7462,7 +7465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -7665,7 +7668,7 @@
         <v>486.04735240937902</v>
       </c>
     </row>
-    <row r="29" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -7868,7 +7871,7 @@
         <v>618.39024922524004</v>
       </c>
     </row>
-    <row r="30" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -8071,7 +8074,7 @@
         <v>356.78274269611802</v>
       </c>
     </row>
-    <row r="31" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -8274,7 +8277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -8477,7 +8480,7 @@
         <v>1388.3473873898199</v>
       </c>
     </row>
-    <row r="33" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -8680,7 +8683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -8883,7 +8886,7 @@
         <v>892.34409305731401</v>
       </c>
     </row>
-    <row r="35" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -9086,7 +9089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -9289,7 +9292,7 @@
         <v>680.51726658672897</v>
       </c>
     </row>
-    <row r="37" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -9492,7 +9495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -9695,7 +9698,7 @@
         <v>2691.65696787653</v>
       </c>
     </row>
-    <row r="39" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -9898,7 +9901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -10101,7 +10104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -10304,7 +10307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -10507,7 +10510,7 @@
         <v>697.94180214607798</v>
       </c>
     </row>
-    <row r="43" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -10710,7 +10713,7 @@
         <v>337.43806353841501</v>
       </c>
     </row>
-    <row r="44" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -10913,7 +10916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -11116,7 +11119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -11319,7 +11322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -11522,7 +11525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -11725,7 +11728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -11928,7 +11931,7 @@
         <v>8706.8651795931492</v>
       </c>
     </row>
-    <row r="50" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -12131,7 +12134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -12334,7 +12337,7 @@
         <v>3458.1600312657001</v>
       </c>
     </row>
-    <row r="52" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -12537,7 +12540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -12740,7 +12743,7 @@
         <v>264.89331304905699</v>
       </c>
     </row>
-    <row r="54" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -12943,7 +12946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>54</v>
       </c>
@@ -13146,7 +13149,7 @@
         <v>1543.7872399594</v>
       </c>
     </row>
-    <row r="56" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>55</v>
       </c>
@@ -13349,7 +13352,7 @@
         <v>332.08499716323701</v>
       </c>
     </row>
-    <row r="57" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>56</v>
       </c>
@@ -13552,7 +13555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>57</v>
       </c>
@@ -13755,7 +13758,7 @@
         <v>17519.683688842699</v>
       </c>
     </row>
-    <row r="59" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>58</v>
       </c>
@@ -13958,7 +13961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>59</v>
       </c>
@@ -14161,7 +14164,7 @@
         <v>138.51473497060601</v>
       </c>
     </row>
-    <row r="61" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>60</v>
       </c>
@@ -14364,7 +14367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>61</v>
       </c>
@@ -14567,7 +14570,7 @@
         <v>449.106899680271</v>
       </c>
     </row>
-    <row r="63" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>62</v>
       </c>
@@ -14770,7 +14773,7 @@
         <v>4241.3876741100703</v>
       </c>
     </row>
-    <row r="64" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>63</v>
       </c>
@@ -14973,7 +14976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>64</v>
       </c>
@@ -15176,7 +15179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>65</v>
       </c>
@@ -15379,7 +15382,7 @@
         <v>17646.553489145801</v>
       </c>
     </row>
-    <row r="67" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>66</v>
       </c>
@@ -15582,7 +15585,7 @@
         <v>1140.7094175949001</v>
       </c>
     </row>
-    <row r="68" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>67</v>
       </c>
@@ -15785,7 +15788,7 @@
         <v>1505.7900985010001</v>
       </c>
     </row>
-    <row r="69" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>68</v>
       </c>
@@ -15988,7 +15991,7 @@
         <v>13850.1879496485</v>
       </c>
     </row>
-    <row r="70" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>69</v>
       </c>
@@ -16191,7 +16194,7 @@
         <v>1823.1525811152601</v>
       </c>
     </row>
-    <row r="71" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>70</v>
       </c>
@@ -16394,7 +16397,7 @@
         <v>313.50014071730601</v>
       </c>
     </row>
-    <row r="72" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>71</v>
       </c>
@@ -16597,7 +16600,7 @@
         <v>3551.8223665741698</v>
       </c>
     </row>
-    <row r="73" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>72</v>
       </c>
@@ -16800,7 +16803,7 @@
         <v>3432.0984867891498</v>
       </c>
     </row>
-    <row r="74" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>73</v>
       </c>
@@ -17003,7 +17006,7 @@
         <v>6358.3530343816401</v>
       </c>
     </row>
-    <row r="75" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>74</v>
       </c>
@@ -17206,7 +17209,7 @@
         <v>62305.686333577403</v>
       </c>
     </row>
-    <row r="76" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>75</v>
       </c>
@@ -17409,7 +17412,7 @@
         <v>5111.3281649943101</v>
       </c>
     </row>
-    <row r="77" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>76</v>
       </c>
@@ -17612,7 +17615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>77</v>
       </c>
@@ -17815,7 +17818,7 @@
         <v>14767.775465967399</v>
       </c>
     </row>
-    <row r="79" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>78</v>
       </c>
@@ -18018,7 +18021,7 @@
         <v>1272.29745831331</v>
       </c>
     </row>
-    <row r="80" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>79</v>
       </c>
@@ -18221,7 +18224,7 @@
         <v>15156.904218314799</v>
       </c>
     </row>
-    <row r="81" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>80</v>
       </c>
@@ -18424,7 +18427,7 @@
         <v>14840.233909017999</v>
       </c>
     </row>
-    <row r="82" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>81</v>
       </c>
@@ -18627,7 +18630,7 @@
         <v>35926.062037467702</v>
       </c>
     </row>
-    <row r="83" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>82</v>
       </c>
@@ -18830,7 +18833,7 @@
         <v>2751.6654757453198</v>
       </c>
     </row>
-    <row r="84" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>83</v>
       </c>
@@ -19033,7 +19036,7 @@
         <v>325.98093218034199</v>
       </c>
     </row>
-    <row r="85" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>84</v>
       </c>
@@ -19236,7 +19239,7 @@
         <v>603.72165180495699</v>
       </c>
     </row>
-    <row r="86" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>85</v>
       </c>
@@ -19439,7 +19442,7 @@
         <v>608.351424925022</v>
       </c>
     </row>
-    <row r="87" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>86</v>
       </c>
@@ -19642,7 +19645,7 @@
         <v>93.201175953832802</v>
       </c>
     </row>
-    <row r="88" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>87</v>
       </c>
@@ -19845,7 +19848,7 @@
         <v>472.508372973203</v>
       </c>
     </row>
-    <row r="89" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>88</v>
       </c>
@@ -20048,7 +20051,7 @@
         <v>1371.1094182618001</v>
       </c>
     </row>
-    <row r="90" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>89</v>
       </c>
@@ -20251,7 +20254,7 @@
         <v>142.82574837293799</v>
       </c>
     </row>
-    <row r="91" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>90</v>
       </c>
@@ -20454,7 +20457,7 @@
         <v>1353.2229560498399</v>
       </c>
     </row>
-    <row r="92" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>91</v>
       </c>
@@ -20657,7 +20660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>92</v>
       </c>
@@ -20860,7 +20863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>93</v>
       </c>
@@ -21063,7 +21066,7 @@
         <v>110.35992058511199</v>
       </c>
     </row>
-    <row r="95" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>94</v>
       </c>
@@ -21266,7 +21269,7 @@
         <v>2286.7554274911499</v>
       </c>
     </row>
-    <row r="96" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>95</v>
       </c>
@@ -21469,7 +21472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>96</v>
       </c>
@@ -21672,7 +21675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>97</v>
       </c>
@@ -21875,7 +21878,7 @@
         <v>130.065592172029</v>
       </c>
     </row>
-    <row r="99" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>98</v>
       </c>
@@ -22078,7 +22081,7 @@
         <v>1452.1493120575699</v>
       </c>
     </row>
-    <row r="100" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>99</v>
       </c>
@@ -22281,7 +22284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>100</v>
       </c>
@@ -22484,7 +22487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>101</v>
       </c>
@@ -22687,7 +22690,7 @@
         <v>739.27255783596001</v>
       </c>
     </row>
-    <row r="103" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>102</v>
       </c>
@@ -22890,7 +22893,7 @@
         <v>50.927974932497797</v>
       </c>
     </row>
-    <row r="104" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>103</v>
       </c>
@@ -23093,7 +23096,7 @@
         <v>13.377468700583201</v>
       </c>
     </row>
-    <row r="105" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>104</v>
       </c>
@@ -23296,7 +23299,7 @@
         <v>279.97424761241399</v>
       </c>
     </row>
-    <row r="106" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>105</v>
       </c>
@@ -23499,7 +23502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>106</v>
       </c>
@@ -23702,7 +23705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>107</v>
       </c>
@@ -23905,7 +23908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>108</v>
       </c>
@@ -24108,7 +24111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>109</v>
       </c>
@@ -24311,7 +24314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>110</v>
       </c>
@@ -24514,7 +24517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>111</v>
       </c>
@@ -24717,7 +24720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>112</v>
       </c>
@@ -24920,7 +24923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>113</v>
       </c>
@@ -25123,7 +25126,7 @@
         <v>321.98918826926501</v>
       </c>
     </row>
-    <row r="115" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>114</v>
       </c>
@@ -25326,7 +25329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>115</v>
       </c>
@@ -25529,7 +25532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>116</v>
       </c>
@@ -25732,7 +25735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>117</v>
       </c>
@@ -25935,7 +25938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>118</v>
       </c>
@@ -26138,7 +26141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>119</v>
       </c>
@@ -26341,7 +26344,7 @@
         <v>61.416259046817302</v>
       </c>
     </row>
-    <row r="121" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>120</v>
       </c>
@@ -26544,7 +26547,7 @@
         <v>582.11036555987005</v>
       </c>
     </row>
-    <row r="122" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>121</v>
       </c>
@@ -26747,7 +26750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>122</v>
       </c>
@@ -26950,7 +26953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>123</v>
       </c>
@@ -27153,7 +27156,7 @@
         <v>255.42937936167201</v>
       </c>
     </row>
-    <row r="125" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>124</v>
       </c>
@@ -27356,7 +27359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>125</v>
       </c>
@@ -27559,7 +27562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>126</v>
       </c>
@@ -27762,7 +27765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>127</v>
       </c>
@@ -27965,7 +27968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>128</v>
       </c>
@@ -28168,7 +28171,7 @@
         <v>4327.7978403841498</v>
       </c>
     </row>
-    <row r="130" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>129</v>
       </c>
@@ -28371,7 +28374,7 @@
         <v>82.782923958903297</v>
       </c>
     </row>
-    <row r="131" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>130</v>
       </c>
@@ -28574,7 +28577,7 @@
         <v>2925.0521218946301</v>
       </c>
     </row>
-    <row r="132" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>131</v>
       </c>
@@ -28777,7 +28780,7 @@
         <v>1752.1874789247299</v>
       </c>
     </row>
-    <row r="133" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>132</v>
       </c>
@@ -28980,7 +28983,7 @@
         <v>4906.4264287528504</v>
       </c>
     </row>
-    <row r="134" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>133</v>
       </c>
@@ -29183,7 +29186,7 @@
         <v>543.73997221385503</v>
       </c>
     </row>
-    <row r="135" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>134</v>
       </c>
@@ -29386,7 +29389,7 @@
         <v>1094.9013667711999</v>
       </c>
     </row>
-    <row r="136" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>135</v>
       </c>
@@ -29589,7 +29592,7 @@
         <v>2269.0934189238901</v>
       </c>
     </row>
-    <row r="137" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>136</v>
       </c>
@@ -29792,7 +29795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>137</v>
       </c>
@@ -29995,7 +29998,7 @@
         <v>92.586164954036605</v>
       </c>
     </row>
-    <row r="139" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>138</v>
       </c>
@@ -30198,7 +30201,7 @@
         <v>7094.7483601152098</v>
       </c>
     </row>
-    <row r="140" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>139</v>
       </c>
@@ -30401,7 +30404,7 @@
         <v>1705.4305313116599</v>
       </c>
     </row>
-    <row r="141" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>140</v>
       </c>
@@ -30604,7 +30607,7 @@
         <v>829.99726650300602</v>
       </c>
     </row>
-    <row r="142" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>141</v>
       </c>
@@ -30807,7 +30810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>142</v>
       </c>
@@ -31010,7 +31013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>143</v>
       </c>
@@ -31213,7 +31216,7 @@
         <v>925.27756076601304</v>
       </c>
     </row>
-    <row r="145" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>144</v>
       </c>
@@ -31416,7 +31419,7 @@
         <v>7379.8117538382903</v>
       </c>
     </row>
-    <row r="146" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>145</v>
       </c>
@@ -31619,7 +31622,7 @@
         <v>8600.9387740935508</v>
       </c>
     </row>
-    <row r="147" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>146</v>
       </c>
@@ -31822,7 +31825,7 @@
         <v>15448.4448573725</v>
       </c>
     </row>
-    <row r="148" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>147</v>
       </c>
@@ -32025,7 +32028,7 @@
         <v>725.86442880817697</v>
       </c>
     </row>
-    <row r="149" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>148</v>
       </c>
@@ -32228,7 +32231,7 @@
         <v>577.75257167745997</v>
       </c>
     </row>
-    <row r="150" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>149</v>
       </c>
@@ -32431,7 +32434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>150</v>
       </c>
@@ -32634,7 +32637,7 @@
         <v>7850.10511986864</v>
       </c>
     </row>
-    <row r="152" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>151</v>
       </c>
@@ -32837,7 +32840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>152</v>
       </c>
@@ -33040,7 +33043,7 @@
         <v>203.68956289888001</v>
       </c>
     </row>
-    <row r="154" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>153</v>
       </c>
@@ -33243,7 +33246,7 @@
         <v>462.93082477018299</v>
       </c>
     </row>
-    <row r="155" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>154</v>
       </c>
@@ -33446,7 +33449,7 @@
         <v>2344.3327933986302</v>
       </c>
     </row>
-    <row r="156" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>155</v>
       </c>
@@ -33649,7 +33652,7 @@
         <v>350.17065290579802</v>
       </c>
     </row>
-    <row r="157" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>156</v>
       </c>
@@ -33852,7 +33855,7 @@
         <v>1030.39923140473</v>
       </c>
     </row>
-    <row r="158" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>157</v>
       </c>
@@ -34055,7 +34058,7 @@
         <v>3650.6660293632599</v>
       </c>
     </row>
-    <row r="159" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>158</v>
       </c>
@@ -34258,7 +34261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>159</v>
       </c>
@@ -34461,7 +34464,7 @@
         <v>184.755587980298</v>
       </c>
     </row>
-    <row r="161" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>160</v>
       </c>
@@ -34664,7 +34667,7 @@
         <v>7470.6711220649304</v>
       </c>
     </row>
-    <row r="162" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>161</v>
       </c>
@@ -34867,7 +34870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>162</v>
       </c>
@@ -35070,7 +35073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>163</v>
       </c>
@@ -35273,7 +35276,7 @@
         <v>6140.1395557645001</v>
       </c>
     </row>
-    <row r="165" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>164</v>
       </c>
@@ -35476,7 +35479,7 @@
         <v>2007.5493690887899</v>
       </c>
     </row>
-    <row r="166" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>165</v>
       </c>
@@ -35679,7 +35682,7 @@
         <v>410.69524751185401</v>
       </c>
     </row>
-    <row r="167" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>166</v>
       </c>
@@ -35882,7 +35885,7 @@
         <v>898.21821856600502</v>
       </c>
     </row>
-    <row r="168" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>167</v>
       </c>
@@ -36085,7 +36088,7 @@
         <v>229.13780903335601</v>
       </c>
     </row>
-    <row r="169" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>168</v>
       </c>
@@ -36288,7 +36291,7 @@
         <v>627.78913858267504</v>
       </c>
     </row>
-    <row r="170" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>169</v>
       </c>
@@ -36491,7 +36494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>170</v>
       </c>
@@ -36694,7 +36697,7 @@
         <v>357.80834305838698</v>
       </c>
     </row>
-    <row r="172" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>171</v>
       </c>
@@ -36897,7 +36900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>172</v>
       </c>
@@ -37100,7 +37103,7 @@
         <v>298.76999642561702</v>
       </c>
     </row>
-    <row r="174" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>173</v>
       </c>
@@ -37303,7 +37306,7 @@
         <v>11196.985667445701</v>
       </c>
     </row>
-    <row r="175" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>174</v>
       </c>
@@ -37506,7 +37509,7 @@
         <v>8211.7323604129397</v>
       </c>
     </row>
-    <row r="176" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>175</v>
       </c>
@@ -37709,7 +37712,7 @@
         <v>402.69968829716902</v>
       </c>
     </row>
-    <row r="177" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>176</v>
       </c>
@@ -37912,7 +37915,7 @@
         <v>4493.94093606563</v>
       </c>
     </row>
-    <row r="178" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>177</v>
       </c>
@@ -38115,7 +38118,7 @@
         <v>875.433999152924</v>
       </c>
     </row>
-    <row r="179" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>178</v>
       </c>
@@ -38318,7 +38321,7 @@
         <v>4485.3588111846102</v>
       </c>
     </row>
-    <row r="180" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>179</v>
       </c>
@@ -38521,7 +38524,7 @@
         <v>14522.1610063894</v>
       </c>
     </row>
-    <row r="181" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>180</v>
       </c>
@@ -38724,7 +38727,7 @@
         <v>454.43774019447102</v>
       </c>
     </row>
-    <row r="182" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>181</v>
       </c>
@@ -38927,7 +38930,7 @@
         <v>3244.6273730728399</v>
       </c>
     </row>
-    <row r="183" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>182</v>
       </c>
@@ -39130,7 +39133,7 @@
         <v>2647.8582815622299</v>
       </c>
     </row>
-    <row r="184" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>183</v>
       </c>
@@ -39333,7 +39336,7 @@
         <v>2347.1660280691499</v>
       </c>
     </row>
-    <row r="185" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>184</v>
       </c>
@@ -39536,7 +39539,7 @@
         <v>5979.04007826407</v>
       </c>
     </row>
-    <row r="186" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>185</v>
       </c>
@@ -39739,7 +39742,7 @@
         <v>5594.0581648018597</v>
       </c>
     </row>
-    <row r="187" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>186</v>
       </c>
@@ -39942,7 +39945,7 @@
         <v>94.813936006828598</v>
       </c>
     </row>
-    <row r="188" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>187</v>
       </c>
@@ -40145,7 +40148,7 @@
         <v>877.86777927396395</v>
       </c>
     </row>
-    <row r="189" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>188</v>
       </c>
@@ -40348,7 +40351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>189</v>
       </c>
@@ -40551,7 +40554,7 @@
         <v>1139.2858891825599</v>
       </c>
     </row>
-    <row r="191" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>190</v>
       </c>
@@ -40754,7 +40757,7 @@
         <v>215.61496336680699</v>
       </c>
     </row>
-    <row r="192" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>191</v>
       </c>
@@ -40957,7 +40960,7 @@
         <v>523.40714248348502</v>
       </c>
     </row>
-    <row r="193" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>192</v>
       </c>
@@ -41160,7 +41163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>193</v>
       </c>
@@ -41363,7 +41366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>194</v>
       </c>
@@ -41566,7 +41569,7 @@
         <v>8887.8961715608802</v>
       </c>
     </row>
-    <row r="196" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>195</v>
       </c>
@@ -41769,7 +41772,7 @@
         <v>1363.2086535368601</v>
       </c>
     </row>
-    <row r="197" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>196</v>
       </c>
@@ -41972,7 +41975,7 @@
         <v>160.04580350669099</v>
       </c>
     </row>
-    <row r="198" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>197</v>
       </c>
@@ -42175,7 +42178,7 @@
         <v>7024.5445562419</v>
       </c>
     </row>
-    <row r="199" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>198</v>
       </c>
@@ -42378,7 +42381,7 @@
         <v>4977.5067726973903</v>
       </c>
     </row>
-    <row r="200" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>199</v>
       </c>
@@ -42581,7 +42584,7 @@
         <v>2488.1299102886601</v>
       </c>
     </row>
-    <row r="201" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>200</v>
       </c>
@@ -42784,7 +42787,7 @@
         <v>4120.1292332144303</v>
       </c>
     </row>
-    <row r="202" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>201</v>
       </c>
@@ -42987,7 +42990,7 @@
         <v>2537.9165103270502</v>
       </c>
     </row>
-    <row r="203" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>202</v>
       </c>
@@ -43190,7 +43193,7 @@
         <v>4889.5050783975003</v>
       </c>
     </row>
-    <row r="204" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>203</v>
       </c>
@@ -43393,7 +43396,7 @@
         <v>197.27405044285999</v>
       </c>
     </row>
-    <row r="205" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>204</v>
       </c>
@@ -43596,7 +43599,7 @@
         <v>1674.4826510672999</v>
       </c>
     </row>
-    <row r="206" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>205</v>
       </c>
@@ -43799,7 +43802,7 @@
         <v>87.1399199567403</v>
       </c>
     </row>
-    <row r="207" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>206</v>
       </c>
@@ -44002,7 +44005,7 @@
         <v>2281.1103538311399</v>
       </c>
     </row>
-    <row r="208" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>207</v>
       </c>
@@ -44205,7 +44208,7 @@
         <v>156.15086904869401</v>
       </c>
     </row>
-    <row r="209" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>208</v>
       </c>
@@ -44408,7 +44411,7 @@
         <v>1556.5510141925799</v>
       </c>
     </row>
-    <row r="210" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>209</v>
       </c>
@@ -44611,7 +44614,7 @@
         <v>369.14570320393898</v>
       </c>
     </row>
-    <row r="211" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>210</v>
       </c>
@@ -44814,7 +44817,7 @@
         <v>165.46339380399601</v>
       </c>
     </row>
-    <row r="212" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>211</v>
       </c>
@@ -45017,7 +45020,7 @@
         <v>147.103986391853</v>
       </c>
     </row>
-    <row r="213" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>212</v>
       </c>
@@ -45220,7 +45223,7 @@
         <v>1766.5428909949401</v>
       </c>
     </row>
-    <row r="214" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>213</v>
       </c>
@@ -45423,7 +45426,7 @@
         <v>2382.4171800581198</v>
       </c>
     </row>
-    <row r="215" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>214</v>
       </c>
@@ -45626,7 +45629,7 @@
         <v>510.78134741302301</v>
       </c>
     </row>
-    <row r="216" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>215</v>
       </c>
@@ -45829,7 +45832,7 @@
         <v>2252.38892655882</v>
       </c>
     </row>
-    <row r="217" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>216</v>
       </c>
@@ -46032,7 +46035,7 @@
         <v>253.82339410244899</v>
       </c>
     </row>
-    <row r="218" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>217</v>
       </c>
@@ -46235,7 +46238,7 @@
         <v>148.472295021592</v>
       </c>
     </row>
-    <row r="219" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>218</v>
       </c>
@@ -46438,7 +46441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>219</v>
       </c>
@@ -46641,7 +46644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>220</v>
       </c>
@@ -46844,7 +46847,7 @@
         <v>1332.7223708187</v>
       </c>
     </row>
-    <row r="222" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>221</v>
       </c>
@@ -47047,7 +47050,7 @@
         <v>1252.68850707878</v>
       </c>
     </row>
-    <row r="223" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>222</v>
       </c>
@@ -47250,7 +47253,7 @@
         <v>470.956098215488</v>
       </c>
     </row>
-    <row r="224" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>223</v>
       </c>
@@ -47453,7 +47456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>224</v>
       </c>
@@ -47656,7 +47659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>225</v>
       </c>
@@ -47859,7 +47862,7 @@
         <v>343.13576857606199</v>
       </c>
     </row>
-    <row r="227" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>226</v>
       </c>
@@ -48062,7 +48065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>227</v>
       </c>
@@ -48265,7 +48268,7 @@
         <v>670.13525588399204</v>
       </c>
     </row>
-    <row r="229" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>228</v>
       </c>
@@ -48468,7 +48471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>229</v>
       </c>
@@ -48671,7 +48674,7 @@
         <v>3043.83326199976</v>
       </c>
     </row>
-    <row r="231" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>230</v>
       </c>
@@ -48874,7 +48877,7 @@
         <v>42.775371042594401</v>
       </c>
     </row>
-    <row r="232" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>231</v>
       </c>
@@ -49077,7 +49080,7 @@
         <v>382.75342926482301</v>
       </c>
     </row>
-    <row r="233" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>232</v>
       </c>
@@ -49280,7 +49283,7 @@
         <v>1606.1519901945501</v>
       </c>
     </row>
-    <row r="234" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>233</v>
       </c>
@@ -49483,7 +49486,7 @@
         <v>1215.44517969761</v>
       </c>
     </row>
-    <row r="235" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>234</v>
       </c>
@@ -49686,7 +49689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>235</v>
       </c>
@@ -49889,7 +49892,7 @@
         <v>642.30493982193195</v>
       </c>
     </row>
-    <row r="237" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>236</v>
       </c>
@@ -50092,7 +50095,7 @@
         <v>81.049250158716902</v>
       </c>
     </row>
-    <row r="238" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>237</v>
       </c>
@@ -50295,7 +50298,7 @@
         <v>3379.3701143673602</v>
       </c>
     </row>
-    <row r="239" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>238</v>
       </c>
@@ -50498,7 +50501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
         <v>239</v>
       </c>
@@ -50701,7 +50704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>240</v>
       </c>
@@ -50904,7 +50907,7 @@
         <v>46.599659182164103</v>
       </c>
     </row>
-    <row r="242" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>241</v>
       </c>
@@ -51107,7 +51110,7 @@
         <v>86.9840092346316</v>
       </c>
     </row>
-    <row r="243" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
         <v>242</v>
       </c>
@@ -51310,7 +51313,7 @@
         <v>196.496232917047</v>
       </c>
     </row>
-    <row r="244" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>243</v>
       </c>
@@ -51513,7 +51516,7 @@
         <v>85.942577545120997</v>
       </c>
     </row>
-    <row r="245" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>244</v>
       </c>
@@ -51716,7 +51719,7 @@
         <v>1631.1677284769901</v>
       </c>
     </row>
-    <row r="246" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>245</v>
       </c>
@@ -51919,7 +51922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>246</v>
       </c>
@@ -52122,7 +52125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
         <v>247</v>
       </c>
@@ -52325,7 +52328,7 @@
         <v>206.14888290547199</v>
       </c>
     </row>
-    <row r="249" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>248</v>
       </c>
@@ -52528,7 +52531,7 @@
         <v>5857.5433864193001</v>
       </c>
     </row>
-    <row r="250" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
         <v>249</v>
       </c>
@@ -52731,7 +52734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="251" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>250</v>
       </c>
@@ -52934,7 +52937,7 @@
         <v>2034.1342996606099</v>
       </c>
     </row>
-    <row r="252" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>251</v>
       </c>
@@ -53137,7 +53140,7 @@
         <v>210.042105390703</v>
       </c>
     </row>
-    <row r="253" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
         <v>252</v>
       </c>
@@ -53340,7 +53343,7 @@
         <v>3441.13684426583</v>
       </c>
     </row>
-    <row r="254" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>253</v>
       </c>
@@ -53543,7 +53546,7 @@
         <v>170.41086263992199</v>
       </c>
     </row>
-    <row r="255" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>254</v>
       </c>
@@ -53746,7 +53749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="256" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>255</v>
       </c>
@@ -53949,7 +53952,7 @@
         <v>113.18844830842001</v>
       </c>
     </row>
-    <row r="257" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>256</v>
       </c>
@@ -54152,7 +54155,7 @@
         <v>405.74429640964797</v>
       </c>
     </row>
-    <row r="258" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>257</v>
       </c>
@@ -54355,7 +54358,7 @@
         <v>555.82017143790495</v>
       </c>
     </row>
-    <row r="259" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
         <v>258</v>
       </c>
@@ -54558,7 +54561,7 @@
         <v>3627.6491676472801</v>
       </c>
     </row>
-    <row r="260" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>259</v>
       </c>
@@ -54761,7 +54764,7 @@
         <v>1958.3561251134399</v>
       </c>
     </row>
-    <row r="261" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
         <v>260</v>
       </c>
@@ -54964,7 +54967,7 @@
         <v>493.28483700166697</v>
       </c>
     </row>
-    <row r="262" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
         <v>261</v>
       </c>
@@ -55167,7 +55170,7 @@
         <v>721.181414613372</v>
       </c>
     </row>
-    <row r="263" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
         <v>262</v>
       </c>
@@ -55370,7 +55373,7 @@
         <v>868.29619655192096</v>
       </c>
     </row>
-    <row r="264" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
         <v>263</v>
       </c>
@@ -55573,7 +55576,7 @@
         <v>282.48917482326499</v>
       </c>
     </row>
-    <row r="265" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
         <v>264</v>
       </c>
@@ -55776,7 +55779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
         <v>265</v>
       </c>
@@ -55979,7 +55982,7 @@
         <v>3330.0030493996201</v>
       </c>
     </row>
-    <row r="267" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
         <v>266</v>
       </c>
@@ -56182,7 +56185,7 @@
         <v>5006.1277428530102</v>
       </c>
     </row>
-    <row r="268" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
         <v>267</v>
       </c>
@@ -56385,7 +56388,7 @@
         <v>7096.7149209768004</v>
       </c>
     </row>
-    <row r="269" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
         <v>268</v>
       </c>
@@ -56588,7 +56591,7 @@
         <v>371.23813702670401</v>
       </c>
     </row>
-    <row r="270" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
         <v>269</v>
       </c>
@@ -56791,7 +56794,7 @@
         <v>574.85568349626703</v>
       </c>
     </row>
-    <row r="271" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
         <v>270</v>
       </c>
@@ -56994,7 +56997,7 @@
         <v>1340.3392014439901</v>
       </c>
     </row>
-    <row r="272" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
         <v>271</v>
       </c>
@@ -57197,7 +57200,7 @@
         <v>193.95182335378701</v>
       </c>
     </row>
-    <row r="273" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
         <v>272</v>
       </c>
@@ -57400,7 +57403,7 @@
         <v>921.12312827904498</v>
       </c>
     </row>
-    <row r="274" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
         <v>273</v>
       </c>
@@ -57603,7 +57606,7 @@
         <v>247.99480686833701</v>
       </c>
     </row>
-    <row r="275" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
         <v>274</v>
       </c>
@@ -57806,7 +57809,7 @@
         <v>88.324877027281801</v>
       </c>
     </row>
-    <row r="276" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
         <v>275</v>
       </c>
@@ -58009,7 +58012,7 @@
         <v>10352.528067360099</v>
       </c>
     </row>
-    <row r="277" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
         <v>276</v>
       </c>
@@ -58212,7 +58215,7 @@
         <v>385.977451327697</v>
       </c>
     </row>
-    <row r="278" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
         <v>277</v>
       </c>
@@ -58415,7 +58418,7 @@
         <v>349.64332546163303</v>
       </c>
     </row>
-    <row r="279" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
         <v>278</v>
       </c>
@@ -58618,7 +58621,7 @@
         <v>2763.7433601929702</v>
       </c>
     </row>
-    <row r="280" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
         <v>279</v>
       </c>
@@ -58821,7 +58824,7 @@
         <v>3425.68181469194</v>
       </c>
     </row>
-    <row r="281" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
         <v>280</v>
       </c>
@@ -59024,7 +59027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="282" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
         <v>281</v>
       </c>
@@ -59227,7 +59230,7 @@
         <v>3110.80383915733</v>
       </c>
     </row>
-    <row r="283" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
         <v>282</v>
       </c>
@@ -59430,7 +59433,7 @@
         <v>4699.0745225426599</v>
       </c>
     </row>
-    <row r="284" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
         <v>283</v>
       </c>
@@ -59633,7 +59636,7 @@
         <v>88.232583529865593</v>
       </c>
     </row>
-    <row r="285" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
         <v>284</v>
       </c>
@@ -59836,7 +59839,7 @@
         <v>3938.8975157619102</v>
       </c>
     </row>
-    <row r="286" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
         <v>285</v>
       </c>
@@ -60039,7 +60042,7 @@
         <v>2393.4889245823201</v>
       </c>
     </row>
-    <row r="287" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
         <v>286</v>
       </c>
@@ -60242,7 +60245,7 @@
         <v>1835.62135734959</v>
       </c>
     </row>
-    <row r="288" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
         <v>287</v>
       </c>
@@ -60445,7 +60448,7 @@
         <v>9614.1103794107094</v>
       </c>
     </row>
-    <row r="289" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
         <v>288</v>
       </c>
@@ -60648,7 +60651,7 @@
         <v>360.21776485024901</v>
       </c>
     </row>
-    <row r="290" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
         <v>289</v>
       </c>
@@ -60851,7 +60854,7 @@
         <v>3088.1831703836401</v>
       </c>
     </row>
-    <row r="291" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
         <v>290</v>
       </c>
@@ -61054,7 +61057,7 @@
         <v>1019.1190489614499</v>
       </c>
     </row>
-    <row r="292" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
         <v>291</v>
       </c>
@@ -61257,7 +61260,7 @@
         <v>92.128251689505404</v>
       </c>
     </row>
-    <row r="293" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
         <v>292</v>
       </c>
@@ -61460,7 +61463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="294" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
         <v>293</v>
       </c>
@@ -61663,7 +61666,7 @@
         <v>4020.7944873259198</v>
       </c>
     </row>
-    <row r="295" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
         <v>294</v>
       </c>
@@ -61866,7 +61869,7 @@
         <v>3685.1645443811699</v>
       </c>
     </row>
-    <row r="296" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
         <v>295</v>
       </c>
@@ -62069,7 +62072,7 @@
         <v>847.86958307548798</v>
       </c>
     </row>
-    <row r="297" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
         <v>296</v>
       </c>
@@ -62272,7 +62275,7 @@
         <v>9754.2964428728992</v>
       </c>
     </row>
-    <row r="298" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
         <v>297</v>
       </c>
@@ -62475,7 +62478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="299" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
         <v>298</v>
       </c>
@@ -62678,7 +62681,7 @@
         <v>213.708448240363</v>
       </c>
     </row>
-    <row r="300" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
         <v>299</v>
       </c>
@@ -62881,7 +62884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="301" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
         <v>300</v>
       </c>
@@ -63084,7 +63087,7 @@
         <v>276.76896899382803</v>
       </c>
     </row>
-    <row r="302" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
         <v>301</v>
       </c>
@@ -63287,7 +63290,7 @@
         <v>503.11760239525398</v>
       </c>
     </row>
-    <row r="303" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
         <v>302</v>
       </c>
@@ -63490,7 +63493,7 @@
         <v>629.97805211289995</v>
       </c>
     </row>
-    <row r="304" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
         <v>303</v>
       </c>
@@ -63693,7 +63696,7 @@
         <v>1117.2517088229499</v>
       </c>
     </row>
-    <row r="305" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
         <v>304</v>
       </c>
@@ -63896,7 +63899,7 @@
         <v>1319.4963214245599</v>
       </c>
     </row>
-    <row r="306" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
         <v>305</v>
       </c>
@@ -64099,7 +64102,7 @@
         <v>342.85890112048997</v>
       </c>
     </row>
-    <row r="307" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
         <v>306</v>
       </c>
@@ -64302,7 +64305,7 @@
         <v>2606.37287968791</v>
       </c>
     </row>
-    <row r="308" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
         <v>307</v>
       </c>
@@ -64505,7 +64508,7 @@
         <v>239.77936801550001</v>
       </c>
     </row>
-    <row r="309" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
         <v>308</v>
       </c>
@@ -64708,7 +64711,7 @@
         <v>1690.96124143417</v>
       </c>
     </row>
-    <row r="310" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
         <v>309</v>
       </c>
@@ -64911,7 +64914,7 @@
         <v>832.99349758412995</v>
       </c>
     </row>
-    <row r="311" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
         <v>310</v>
       </c>
@@ -65114,7 +65117,7 @@
         <v>191.73156775222799</v>
       </c>
     </row>
-    <row r="312" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
         <v>311</v>
       </c>
@@ -65317,7 +65320,7 @@
         <v>2798.42241690232</v>
       </c>
     </row>
-    <row r="313" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
         <v>312</v>
       </c>
@@ -65520,7 +65523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="314" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
         <v>313</v>
       </c>
@@ -65723,7 +65726,7 @@
         <v>278.88759443471997</v>
       </c>
     </row>
-    <row r="315" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
         <v>314</v>
       </c>
@@ -65926,7 +65929,7 @@
         <v>157.449972725181</v>
       </c>
     </row>
-    <row r="316" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
         <v>315</v>
       </c>
@@ -66129,7 +66132,7 @@
         <v>307.84899847217099</v>
       </c>
     </row>
-    <row r="317" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
         <v>316</v>
       </c>
@@ -66332,7 +66335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="318" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
         <v>317</v>
       </c>
@@ -66535,7 +66538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="319" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
         <v>318</v>
       </c>
@@ -66738,7 +66741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="320" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A320" t="s">
         <v>319</v>
       </c>
@@ -66941,7 +66944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="321" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
         <v>320</v>
       </c>
@@ -67144,7 +67147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="322" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
         <v>321</v>
       </c>
@@ -67347,7 +67350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="323" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A323" t="s">
         <v>322</v>
       </c>
@@ -67550,7 +67553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="324" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
         <v>323</v>
       </c>
@@ -67753,7 +67756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="325" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
         <v>324</v>
       </c>
@@ -67956,7 +67959,7 @@
         <v>318.71039969639298</v>
       </c>
     </row>
-    <row r="326" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
         <v>325</v>
       </c>
@@ -68159,7 +68162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="327" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A327" t="s">
         <v>326</v>
       </c>
@@ -68362,7 +68365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="328" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A328" t="s">
         <v>327</v>
       </c>
@@ -68565,7 +68568,7 @@
         <v>74.362468021207704</v>
       </c>
     </row>
-    <row r="329" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A329" t="s">
         <v>328</v>
       </c>
@@ -68768,7 +68771,7 @@
         <v>72.275626934038797</v>
       </c>
     </row>
-    <row r="330" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A330" t="s">
         <v>329</v>
       </c>
@@ -68971,7 +68974,7 @@
         <v>83.990632398621997</v>
       </c>
     </row>
-    <row r="331" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A331" t="s">
         <v>330</v>
       </c>
@@ -69174,7 +69177,7 @@
         <v>56.695556695220198</v>
       </c>
     </row>
-    <row r="332" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A332" t="s">
         <v>331</v>
       </c>
@@ -69377,7 +69380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="333" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A333" t="s">
         <v>332</v>
       </c>
@@ -69580,7 +69583,7 @@
         <v>22.674162845886499</v>
       </c>
     </row>
-    <row r="334" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A334" t="s">
         <v>333</v>
       </c>
@@ -69783,7 +69786,7 @@
         <v>230.31775001942</v>
       </c>
     </row>
-    <row r="335" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A335" t="s">
         <v>334</v>
       </c>
@@ -69986,7 +69989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="336" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A336" t="s">
         <v>335</v>
       </c>
@@ -70189,7 +70192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="337" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A337" t="s">
         <v>336</v>
       </c>
@@ -70392,7 +70395,7 @@
         <v>34.2689052102603</v>
       </c>
     </row>
-    <row r="338" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A338" t="s">
         <v>337</v>
       </c>
@@ -70595,7 +70598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="339" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A339" t="s">
         <v>338</v>
       </c>
@@ -70798,7 +70801,7 @@
         <v>1267.8382019814601</v>
       </c>
     </row>
-    <row r="340" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A340" t="s">
         <v>339</v>
       </c>
@@ -71001,7 +71004,7 @@
         <v>411.16332392926699</v>
       </c>
     </row>
-    <row r="341" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A341" t="s">
         <v>340</v>
       </c>
@@ -71204,7 +71207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="342" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A342" t="s">
         <v>341</v>
       </c>
@@ -71407,7 +71410,7 @@
         <v>249.44071481433701</v>
       </c>
     </row>
-    <row r="343" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A343" t="s">
         <v>342</v>
       </c>
@@ -71610,7 +71613,7 @@
         <v>462.32863097746701</v>
       </c>
     </row>
-    <row r="344" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A344" t="s">
         <v>343</v>
       </c>
@@ -71813,7 +71816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="345" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A345" t="s">
         <v>344</v>
       </c>
@@ -72016,7 +72019,7 @@
         <v>192.78215168511699</v>
       </c>
     </row>
-    <row r="346" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A346" t="s">
         <v>345</v>
       </c>
@@ -72219,7 +72222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="347" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A347" t="s">
         <v>346</v>
       </c>
@@ -72422,7 +72425,7 @@
         <v>1722.9351239161099</v>
       </c>
     </row>
-    <row r="348" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A348" t="s">
         <v>347</v>
       </c>
@@ -72626,7 +72629,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="C1:C348" xr:uid="{00755AFE-4DED-7240-89EB-BC10209B4B62}"/>
+  <autoFilter ref="A1:BO348" xr:uid="{00755AFE-4DED-7240-89EB-BC10209B4B62}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>